<commit_message>
feat: adição de funcionalidades e algumas correções
</commit_message>
<xml_diff>
--- a/banco.xlsx
+++ b/banco.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:AJ9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -493,6 +493,131 @@
           <t>Reunião com  Cliente</t>
         </is>
       </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Nº Proposta:</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 12</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Nº Pedido:</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Nº Pedido de Vendas:</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Data Entrada do Pedido:</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Nº Cliente:</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Quantidade:</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Data Entrega Cliente:</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Status, Prazo Compra:</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Status Painel:</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Reunião com Cliente:</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 22</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 23</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>Data Entrada do Pedido</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>Nome</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>Idade</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>DataCadastro</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>Endereço</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>Telefone</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>Cidade</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>Estado</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>País</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>CEP</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>Observações</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -536,6 +661,31 @@
           <t>Não é necessário</t>
         </is>
       </c>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr"/>
+      <c r="X2" t="inlineStr"/>
+      <c r="Y2" t="inlineStr"/>
+      <c r="Z2" t="inlineStr"/>
+      <c r="AA2" t="inlineStr"/>
+      <c r="AB2" t="inlineStr"/>
+      <c r="AC2" t="inlineStr"/>
+      <c r="AD2" t="inlineStr"/>
+      <c r="AE2" t="inlineStr"/>
+      <c r="AF2" t="inlineStr"/>
+      <c r="AG2" t="inlineStr"/>
+      <c r="AH2" t="inlineStr"/>
+      <c r="AI2" t="inlineStr"/>
+      <c r="AJ2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -583,6 +733,31 @@
           <t>110</t>
         </is>
       </c>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="inlineStr"/>
+      <c r="T3" t="inlineStr"/>
+      <c r="U3" t="inlineStr"/>
+      <c r="V3" t="inlineStr"/>
+      <c r="W3" t="inlineStr"/>
+      <c r="X3" t="inlineStr"/>
+      <c r="Y3" t="inlineStr"/>
+      <c r="Z3" t="inlineStr"/>
+      <c r="AA3" t="inlineStr"/>
+      <c r="AB3" t="inlineStr"/>
+      <c r="AC3" t="inlineStr"/>
+      <c r="AD3" t="inlineStr"/>
+      <c r="AE3" t="inlineStr"/>
+      <c r="AF3" t="inlineStr"/>
+      <c r="AG3" t="inlineStr"/>
+      <c r="AH3" t="inlineStr"/>
+      <c r="AI3" t="inlineStr"/>
+      <c r="AJ3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -630,6 +805,31 @@
           <t>11</t>
         </is>
       </c>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
+      <c r="W4" t="inlineStr"/>
+      <c r="X4" t="inlineStr"/>
+      <c r="Y4" t="inlineStr"/>
+      <c r="Z4" t="inlineStr"/>
+      <c r="AA4" t="inlineStr"/>
+      <c r="AB4" t="inlineStr"/>
+      <c r="AC4" t="inlineStr"/>
+      <c r="AD4" t="inlineStr"/>
+      <c r="AE4" t="inlineStr"/>
+      <c r="AF4" t="inlineStr"/>
+      <c r="AG4" t="inlineStr"/>
+      <c r="AH4" t="inlineStr"/>
+      <c r="AI4" t="inlineStr"/>
+      <c r="AJ4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -685,6 +885,331 @@
       <c r="K5" t="inlineStr">
         <is>
           <t>k</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr"/>
+      <c r="R5" t="inlineStr"/>
+      <c r="S5" t="inlineStr"/>
+      <c r="T5" t="inlineStr"/>
+      <c r="U5" t="inlineStr"/>
+      <c r="V5" t="inlineStr"/>
+      <c r="W5" t="inlineStr"/>
+      <c r="X5" t="inlineStr"/>
+      <c r="Y5" t="inlineStr"/>
+      <c r="Z5" t="inlineStr"/>
+      <c r="AA5" t="inlineStr"/>
+      <c r="AB5" t="inlineStr"/>
+      <c r="AC5" t="inlineStr"/>
+      <c r="AD5" t="inlineStr"/>
+      <c r="AE5" t="inlineStr"/>
+      <c r="AF5" t="inlineStr"/>
+      <c r="AG5" t="inlineStr"/>
+      <c r="AH5" t="inlineStr"/>
+      <c r="AI5" t="inlineStr"/>
+      <c r="AJ5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="n">
+        <v>10</v>
+      </c>
+      <c r="M6" t="n">
+        <v>20</v>
+      </c>
+      <c r="N6" t="n">
+        <v>30</v>
+      </c>
+      <c r="O6" t="n">
+        <v>40</v>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>2025-01-29 22:37:43</t>
+        </is>
+      </c>
+      <c r="Q6" t="n">
+        <v>50</v>
+      </c>
+      <c r="R6" t="n">
+        <v>60</v>
+      </c>
+      <c r="S6" t="n">
+        <v>70</v>
+      </c>
+      <c r="T6" t="n">
+        <v>80</v>
+      </c>
+      <c r="U6" t="n">
+        <v>80</v>
+      </c>
+      <c r="V6" t="n">
+        <v>1001</v>
+      </c>
+      <c r="W6" t="inlineStr"/>
+      <c r="X6" t="inlineStr"/>
+      <c r="Y6" t="inlineStr"/>
+      <c r="Z6" t="inlineStr"/>
+      <c r="AA6" t="inlineStr"/>
+      <c r="AB6" t="inlineStr"/>
+      <c r="AC6" t="inlineStr"/>
+      <c r="AD6" t="inlineStr"/>
+      <c r="AE6" t="inlineStr"/>
+      <c r="AF6" t="inlineStr"/>
+      <c r="AG6" t="inlineStr"/>
+      <c r="AH6" t="inlineStr"/>
+      <c r="AI6" t="inlineStr"/>
+      <c r="AJ6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr"/>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="n">
+        <v>10</v>
+      </c>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="n">
+        <v>30</v>
+      </c>
+      <c r="O7" t="n">
+        <v>40</v>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>2025-01-29 22:38:58</t>
+        </is>
+      </c>
+      <c r="Q7" t="n">
+        <v>50</v>
+      </c>
+      <c r="R7" t="n">
+        <v>60</v>
+      </c>
+      <c r="S7" t="n">
+        <v>70</v>
+      </c>
+      <c r="T7" t="n">
+        <v>80</v>
+      </c>
+      <c r="U7" t="n">
+        <v>80</v>
+      </c>
+      <c r="V7" t="n">
+        <v>1001</v>
+      </c>
+      <c r="W7" t="n">
+        <v>20</v>
+      </c>
+      <c r="X7" t="inlineStr"/>
+      <c r="Y7" t="inlineStr"/>
+      <c r="Z7" t="inlineStr"/>
+      <c r="AA7" t="inlineStr"/>
+      <c r="AB7" t="inlineStr"/>
+      <c r="AC7" t="inlineStr"/>
+      <c r="AD7" t="inlineStr"/>
+      <c r="AE7" t="inlineStr"/>
+      <c r="AF7" t="inlineStr"/>
+      <c r="AG7" t="inlineStr"/>
+      <c r="AH7" t="inlineStr"/>
+      <c r="AI7" t="inlineStr"/>
+      <c r="AJ7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr"/>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>v</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>,</t>
+        </is>
+      </c>
+      <c r="V8" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="W8" t="inlineStr"/>
+      <c r="X8" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="Y8" t="inlineStr">
+        <is>
+          <t>2025-01-29 22:39:56</t>
+        </is>
+      </c>
+      <c r="Z8" t="inlineStr"/>
+      <c r="AA8" t="inlineStr"/>
+      <c r="AB8" t="inlineStr"/>
+      <c r="AC8" t="inlineStr"/>
+      <c r="AD8" t="inlineStr"/>
+      <c r="AE8" t="inlineStr"/>
+      <c r="AF8" t="inlineStr"/>
+      <c r="AG8" t="inlineStr"/>
+      <c r="AH8" t="inlineStr"/>
+      <c r="AI8" t="inlineStr"/>
+      <c r="AJ8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr"/>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr"/>
+      <c r="Q9" t="inlineStr"/>
+      <c r="R9" t="inlineStr"/>
+      <c r="S9" t="inlineStr"/>
+      <c r="T9" t="inlineStr"/>
+      <c r="U9" t="inlineStr"/>
+      <c r="V9" t="inlineStr"/>
+      <c r="W9" t="inlineStr"/>
+      <c r="X9" t="inlineStr"/>
+      <c r="Y9" t="inlineStr"/>
+      <c r="Z9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AA9" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AB9" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="AC9" t="inlineStr">
+        <is>
+          <t>2025-01-29 22:41:15</t>
+        </is>
+      </c>
+      <c r="AD9" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="AE9" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="AF9" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="AG9" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="AH9" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="AI9" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="AJ9" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>

</xml_diff>